<commit_message>
Verify search results in excel
</commit_message>
<xml_diff>
--- a/src/test/resources/DataSheet.xlsx
+++ b/src/test/resources/DataSheet.xlsx
@@ -82,7 +82,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -429,9 +428,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -491,7 +488,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>

</xml_diff>